<commit_message>
RQ - AR, aggiornati i requisiti e la descrizione dello UCG 1 secondo correzioni di C. Se non vengono fatte altre modifiche è pronto per la verifica
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RQ/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Funzionali" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="169">
   <si>
     <t>Codice</t>
   </si>
@@ -49,9 +49,6 @@
     <t>interno</t>
   </si>
   <si>
-    <t>Il prodotto non dovrà risentire del traffico presente nella rete</t>
-  </si>
-  <si>
     <t>Capitolato</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>Il sistema dovrà essere funzionale presso aziende diverse, anche con caratteristiche molto differenti fra di loro</t>
   </si>
   <si>
-    <t>Il sistema funzionerà su qualsiasi dispositivo dove è presente una \uline{JVM}  versione &gt;= 7.02</t>
-  </si>
-  <si>
     <t>Il sistema dovrà funzionare su qualsiasi \uline{dispositivo mobile} con sistema operativo \uline{Android}</t>
   </si>
   <si>
@@ -313,12 +307,6 @@
     <t>UCDA 8</t>
   </si>
   <si>
-    <t>RFD .2.2</t>
-  </si>
-  <si>
-    <t>RFOP .2.3</t>
-  </si>
-  <si>
     <t>Un \uline{Amministratore Azienda Autenticato} dovrà avere la possibilità di terminare la propria sessione</t>
   </si>
   <si>
@@ -388,9 +376,6 @@
     <t>UCASA 3.2</t>
   </si>
   <si>
-    <t>Il prodotto dovrà essere prestazionale indipendentemente dalla posizione del server generale delle domande</t>
-  </si>
-  <si>
     <t>Tutti i processi di sviluppo aderiranno allo standard \uline{ISO/IEC} 15504:1998 \uline{SPICE}</t>
   </si>
   <si>
@@ -409,9 +394,6 @@
     <t>Da ogni schermata sarà possibile raggiungere un'area di aiuto che guiderà l'\uline{utilizzatore} spiegandogli le operazioni effettuabili nella pagina in cui esso si trova</t>
   </si>
   <si>
-    <t xml:space="preserve">RVOP </t>
-  </si>
-  <si>
     <t>Un \uline{Amministratore Installatore} potrà installare il software sui \uline{dispositivi fissi} in un'azienda</t>
   </si>
   <si>
@@ -424,9 +406,6 @@
     <t>Sarà fornito un manuale ad uso \uline{Amministratore Installatore} riguardo alle azioni che potrà compiere</t>
   </si>
   <si>
-    <t>Tutte le azioni di tutti gli \uline{utilizzatori}, nel tempo, dovranno essere registrate nel sistema</t>
-  </si>
-  <si>
     <t>RFOB .1.1</t>
   </si>
   <si>
@@ -478,18 +457,12 @@
     <t>Il tipo delle risposte può essere: si/no, risposta chiusa, risposta multipla</t>
   </si>
   <si>
-    <t>Un \uline{Utente} che dovesse aver perso la propria password per accedere al sistema, potrà modificarla</t>
-  </si>
-  <si>
     <t>Un \uline{Utente}, che dovesse aver eseguito correttamente la procedura di modifica password dimenticata, riceverà nella propria casella di posta elettronica una nuova password generata casualmente dal sistema</t>
   </si>
   <si>
     <t>Un \uline{Dipendente} dovrà potersi autenticare nel sistema inserendo le proprie credenziali di accesso</t>
   </si>
   <si>
-    <t>Le domande che verranno sottoposte ai \uline{Dipendenti Autenticati} dovranno poter avere risposta direttamente dalla propria postazione di lavoro</t>
-  </si>
-  <si>
     <t xml:space="preserve">Le domande a cui verranno sottoposti i \uline{Dipendenti Autenticati} forniti di \uline{dispositivi mobili} aziendali potranno prevedere delle prove pratiche </t>
   </si>
   <si>
@@ -509,6 +482,54 @@
   </si>
   <si>
     <t>Un \uline{Amministratore Installatore} avrà la possibilità di creare il database dell'azienda per far funzionare il sistema</t>
+  </si>
+  <si>
+    <t>RFD .1</t>
+  </si>
+  <si>
+    <t>Alcuni obiettivi possono essere: risposto correttamente a 10 domande, risposto a 50 domande, completate tutte le domande a risposta multipla…</t>
+  </si>
+  <si>
+    <t>RFD .1.1</t>
+  </si>
+  <si>
+    <t>Ogni volta che un obiettivo viene completato, il sistema aggiungerà il badge corrispondente al \uline{Dipendente}</t>
+  </si>
+  <si>
+    <t>Un \uline{Utente} che dovesse aver perso la propria password per accedere al sistema, potrà modificarla, inserendo il proprio codice fiscale e username</t>
+  </si>
+  <si>
+    <t>Le domande che verranno sottoposte ai \uline{Dipendenti Autenticati} potranno avere risposta direttamente dalla propria postazione di lavoro</t>
+  </si>
+  <si>
+    <t>RFD .1.2</t>
+  </si>
+  <si>
+    <t>RFOP .1.3</t>
+  </si>
+  <si>
+    <t>RFD .2.1</t>
+  </si>
+  <si>
+    <t>Il prodotto dovrà funzionare indipendentemente dalla posizione del server generale delle domande</t>
+  </si>
+  <si>
+    <t>Il prodotto non dovrà perdere dati, anche con traffico pesante nella rete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RQOP </t>
+  </si>
+  <si>
+    <t>Non sarà possibile che ad un dipendente con un dato impiego (es. segretario) vengano proposte domande riguardanti ambienti che non gli competono (es. sicurezza di macchinari pesanti)</t>
+  </si>
+  <si>
+    <t>Le azioni saranno memorizzate in file di log, diversi per ogni \uline{Utilizzaotre} e diversi per macro tipologia di azione (ad esempio, un file per i login, uno per i logout, uno per le modifiche di password…)</t>
+  </si>
+  <si>
+    <t>Tutte le azioni di tutti gli \uline{Utilizzatori}, nel tempo, dovranno essere registrate nel sistema</t>
+  </si>
+  <si>
+    <t>Il sistema funzionerà su qualsiasi dispositivo dove è presente una \uline{JVM} con release \uline{JSE} versione &gt;= 7.02</t>
   </si>
 </sst>
 </file>
@@ -580,7 +601,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -592,12 +613,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
@@ -909,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -924,936 +946,992 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>147</v>
-      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>50</v>
+      <c r="A16" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>147</v>
+      <c r="C17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>136</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A21" t="s">
-        <v>50</v>
-      </c>
       <c r="B21" s="1" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A24" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30">
-      <c r="A24" t="s">
-        <v>96</v>
-      </c>
       <c r="B24" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>159</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>147</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>160</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>147</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1">
+      <c r="A33" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30">
-      <c r="A32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" t="s">
         <v>85</v>
       </c>
-      <c r="C32" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30">
-      <c r="A34" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" t="s">
-        <v>90</v>
-      </c>
       <c r="D34" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>147</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>159</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>147</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="4" t="s">
-        <v>76</v>
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30">
+      <c r="A40" t="s">
+        <v>48</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
+      </c>
+      <c r="C40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="4" t="s">
-        <v>76</v>
+      <c r="A41" t="s">
+        <v>47</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C42" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" t="s">
-        <v>147</v>
+        <v>150</v>
+      </c>
+      <c r="C41" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C43" t="s">
-        <v>113</v>
-      </c>
-      <c r="D43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1">
-      <c r="A44" t="s">
-        <v>52</v>
+      <c r="A43" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" t="s">
-        <v>147</v>
+        <v>96</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>53</v>
+      <c r="A45" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" t="s">
-        <v>113</v>
-      </c>
-      <c r="D45" t="s">
-        <v>147</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D46" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D47" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" customHeight="1">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D49" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D50" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C51" t="s">
         <v>111</v>
       </c>
       <c r="D51" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D52" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>139</v>
+        <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D53" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="C54" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D54" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C55" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D55" t="s">
-        <v>147</v>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="4" t="s">
-        <v>76</v>
+      <c r="A58" t="s">
+        <v>74</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>147</v>
+        <v>139</v>
+      </c>
+      <c r="C58" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="C59" t="s">
+        <v>95</v>
+      </c>
+      <c r="D59" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D59" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="30">
-      <c r="A60" t="s">
+      <c r="C62" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="30">
+      <c r="A64" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" customHeight="1">
+      <c r="A66" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" customHeight="1">
+      <c r="A67" t="s">
         <v>50</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C60" t="s">
-        <v>37</v>
-      </c>
-      <c r="D60" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>49</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C61" t="s">
-        <v>40</v>
-      </c>
-      <c r="D61" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1">
-      <c r="A62" t="s">
-        <v>50</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C62" t="s">
-        <v>119</v>
-      </c>
-      <c r="D62" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1">
-      <c r="A63" t="s">
-        <v>52</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C63" t="s">
-        <v>120</v>
-      </c>
-      <c r="D63" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>71</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B67" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C67" t="s">
+        <v>116</v>
+      </c>
+      <c r="D67" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" customHeight="1">
+      <c r="A69" t="s">
         <v>137</v>
       </c>
-      <c r="D64" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1">
-      <c r="A65" t="s">
-        <v>144</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C65" t="s">
-        <v>137</v>
-      </c>
-      <c r="D65" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
-        <v>49</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C66" t="s">
-        <v>116</v>
-      </c>
-      <c r="D66" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
-        <v>49</v>
-      </c>
       <c r="B69" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C69" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="D69" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="D70" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" t="s">
-        <v>49</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C71" t="s">
-        <v>10</v>
-      </c>
-      <c r="D71" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" t="s">
-        <v>49</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C72" t="s">
-        <v>10</v>
-      </c>
-      <c r="D72" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1">
+      <c r="A72" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C73" t="s">
+        <v>28</v>
+      </c>
+      <c r="D73" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>47</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B73" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C73" t="s">
-        <v>10</v>
-      </c>
-      <c r="D73" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2">
-      <c r="B97" s="2"/>
+      <c r="C75" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>47</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" customHeight="1">
+      <c r="A77" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A8:D8"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A61:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1867,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1882,30 +1960,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1920,10 +2012,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1934,198 +2026,212 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="D14" t="s">
-        <v>48</v>
+      <c r="D15" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2142,12 +2248,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="112.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -2156,102 +2263,75 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-    </row>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" customHeight="1"/>
     <row r="18" spans="2:2">
       <c r="B18" s="3"/>
     </row>
@@ -2270,7 +2350,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2296,7 +2376,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2310,10 +2390,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato un requisito e messo a posto il tracciamento
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RQ/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Funzionali" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Vincolo" sheetId="4" r:id="rId4"/>
     <sheet name="Formato Tabelle" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -80,9 +80,6 @@
     <t>RVOB .2</t>
   </si>
   <si>
-    <t>Il sistema dovrà funzionare su qualsiasi \uline{dispositivo mobile} con sistema operativo \uline{Android}</t>
-  </si>
-  <si>
     <t>Non si dovranno fare assunzioni sulla locazione dei database delle aziende</t>
   </si>
   <si>
@@ -525,6 +522,9 @@
   </si>
   <si>
     <t>RXY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il sistema dovrà funzionare su qualsiasi \uline{dispositivo mobile} con sistema operativo \uline{Android} la cui versione è &gt;=1.6 e &lt;=4 </t>
   </si>
 </sst>
 </file>
@@ -573,9 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -585,6 +582,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -895,19 +895,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="A1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -918,10 +918,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -932,13 +932,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>61</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -946,13 +946,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -960,13 +960,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -976,19 +976,19 @@
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -999,10 +999,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1012,14 +1012,14 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
-        <v>56</v>
+      <c r="A11" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
         <v>70</v>
-      </c>
-      <c r="C11" t="s">
-        <v>71</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -1027,13 +1027,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -1041,63 +1041,63 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="5" t="s">
+      <c r="B16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1108,10 +1108,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -1122,10 +1122,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1136,13 +1136,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -1150,10 +1150,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1164,10 +1164,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1178,10 +1178,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -1192,10 +1192,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1206,10 +1206,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1220,10 +1220,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -1234,13 +1234,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" t="s">
         <v>93</v>
-      </c>
-      <c r="C28" t="s">
-        <v>94</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -1248,13 +1248,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -1262,10 +1262,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
@@ -1276,10 +1276,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -1290,10 +1290,10 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
@@ -1304,10 +1304,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
@@ -1318,13 +1318,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
         <v>102</v>
-      </c>
-      <c r="C34" t="s">
-        <v>103</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -1332,13 +1332,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -1346,13 +1346,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
         <v>105</v>
-      </c>
-      <c r="C36" t="s">
-        <v>106</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -1360,13 +1360,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -1374,13 +1374,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" t="s">
         <v>108</v>
-      </c>
-      <c r="C38" t="s">
-        <v>109</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -1388,13 +1388,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
         <v>110</v>
-      </c>
-      <c r="C39" t="s">
-        <v>111</v>
       </c>
       <c r="D39" t="s">
         <v>15</v>
@@ -1402,13 +1402,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -1416,13 +1416,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" t="s">
         <v>113</v>
-      </c>
-      <c r="C41" t="s">
-        <v>114</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
@@ -1432,50 +1432,50 @@
       <c r="B42" s="1"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="D44" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" t="s">
         <v>120</v>
-      </c>
-      <c r="C46" t="s">
-        <v>121</v>
       </c>
       <c r="D46" t="s">
         <v>15</v>
@@ -1483,13 +1483,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -1497,13 +1497,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D48" t="s">
         <v>15</v>
@@ -1511,13 +1511,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D49" t="s">
         <v>15</v>
@@ -1525,13 +1525,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="C50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D50" t="s">
         <v>15</v>
@@ -1539,13 +1539,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" t="s">
         <v>128</v>
-      </c>
-      <c r="C51" t="s">
-        <v>129</v>
       </c>
       <c r="D51" t="s">
         <v>15</v>
@@ -1553,13 +1553,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" t="s">
         <v>130</v>
-      </c>
-      <c r="C52" t="s">
-        <v>131</v>
       </c>
       <c r="D52" t="s">
         <v>15</v>
@@ -1567,13 +1567,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
@@ -1581,13 +1581,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" t="s">
         <v>133</v>
-      </c>
-      <c r="C54" t="s">
-        <v>134</v>
       </c>
       <c r="D54" t="s">
         <v>15</v>
@@ -1595,13 +1595,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
@@ -1609,13 +1609,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" t="s">
         <v>136</v>
-      </c>
-      <c r="C56" t="s">
-        <v>137</v>
       </c>
       <c r="D56" t="s">
         <v>15</v>
@@ -1623,13 +1623,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
@@ -1637,13 +1637,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C58" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D58" t="s">
         <v>15</v>
@@ -1651,13 +1651,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" t="s">
         <v>140</v>
-      </c>
-      <c r="C59" t="s">
-        <v>141</v>
       </c>
       <c r="D59" t="s">
         <v>15</v>
@@ -1667,36 +1667,36 @@
       <c r="B60" s="1"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C63" t="s">
         <v>145</v>
-      </c>
-      <c r="C63" t="s">
-        <v>146</v>
       </c>
       <c r="D63" t="s">
         <v>15</v>
@@ -1704,13 +1704,13 @@
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
@@ -1718,13 +1718,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" t="s">
         <v>148</v>
-      </c>
-      <c r="C65" t="s">
-        <v>149</v>
       </c>
       <c r="D65" t="s">
         <v>15</v>
@@ -1732,13 +1732,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C66" t="s">
         <v>150</v>
-      </c>
-      <c r="C66" t="s">
-        <v>151</v>
       </c>
       <c r="D66" t="s">
         <v>15</v>
@@ -1746,13 +1746,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C67" t="s">
         <v>152</v>
-      </c>
-      <c r="C67" t="s">
-        <v>153</v>
       </c>
       <c r="D67" t="s">
         <v>15</v>
@@ -1760,13 +1760,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
+        <v>153</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="C68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D68" t="s">
         <v>15</v>
@@ -1774,13 +1774,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="C69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D69" t="s">
         <v>15</v>
@@ -1788,13 +1788,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C70" t="s">
         <v>158</v>
-      </c>
-      <c r="C70" t="s">
-        <v>159</v>
       </c>
       <c r="D70" t="s">
         <v>15</v>
@@ -1804,22 +1804,22 @@
       <c r="B71" s="1"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="A72" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C73" t="s">
         <v>161</v>
-      </c>
-      <c r="C73" t="s">
-        <v>162</v>
       </c>
       <c r="D73" t="s">
         <v>15</v>
@@ -1827,13 +1827,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C74" t="s">
         <v>163</v>
-      </c>
-      <c r="C74" t="s">
-        <v>164</v>
       </c>
       <c r="D74" t="s">
         <v>15</v>
@@ -1841,10 +1841,10 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C75" t="s">
         <v>18</v>
@@ -1855,10 +1855,10 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C76" t="s">
         <v>18</v>
@@ -1869,10 +1869,10 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>154</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>167</v>
+        <v>153</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>166</v>
       </c>
       <c r="C77" t="s">
         <v>18</v>
@@ -1883,12 +1883,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A72:D72"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A43:D43"/>
     <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A72:D72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1912,13 +1912,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
       </c>
       <c r="D1" t="s">
         <v>15</v>
@@ -1926,13 +1926,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -1976,10 +1976,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -1990,10 +1990,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -2004,10 +2004,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -2018,10 +2018,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -2032,10 +2032,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -2046,10 +2046,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -2060,10 +2060,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -2074,10 +2074,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
         <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -2088,10 +2088,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
         <v>38</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -2102,10 +2102,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -2116,10 +2116,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
         <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -2130,10 +2130,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -2144,10 +2144,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -2172,13 +2172,13 @@
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -2194,14 +2194,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="108.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="122.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2252,7 +2252,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -2266,10 +2266,10 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2284,7 +2284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
RQ: Aggiornati i requisiti e il glossario
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RQ/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Funzionali" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="171">
   <si>
     <t>Codice</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Non si dovranno fare assunzioni sulla locazione dei database delle aziende</t>
   </si>
   <si>
-    <t>Verbale</t>
-  </si>
-  <si>
     <t xml:space="preserve">RQOB </t>
   </si>
   <si>
@@ -107,21 +104,12 @@
     <t>RQOB .2</t>
   </si>
   <si>
-    <t>Sarà fornito un manuale ad uso \uline{Amministratore Azienda}  riguardo tutte le azioni che potrà compiere</t>
-  </si>
-  <si>
     <t>RQOB .3</t>
   </si>
   <si>
-    <t>Sarà fornito un manuale ad uso \uline{Amministratore Installatore} riguardo alle azioni che potrà compiere</t>
-  </si>
-  <si>
     <t>RQOB .4</t>
   </si>
   <si>
-    <t>Sarà fornito un manuale ad uso \uline{Amministratore Sicurezza} riguardo le azioni che potrà compiere</t>
-  </si>
-  <si>
     <t>Le interfacce che saranno visibili ai \uline{Dipendenti} dovranno essere accattivanti e le funzionalità quanto più intuitive, così da invogliare l'utilizzo</t>
   </si>
   <si>
@@ -146,9 +134,6 @@
     <t>Sarà fornita documentazione esaustiva di ogni metodo sviluppato</t>
   </si>
   <si>
-    <t>Le applicazioni \uline{web} aderiranno allo stile \uline{W3C}</t>
-  </si>
-  <si>
     <t>RQD .1</t>
   </si>
   <si>
@@ -173,15 +158,9 @@
     <t>Il prodotto non dovrà perdere dati, anche con traffico pesante nella rete</t>
   </si>
   <si>
-    <t>interno</t>
-  </si>
-  <si>
     <t>Il prodotto dovrà funzionare indipendentemente dalla posizione del server generale delle domande</t>
   </si>
   <si>
-    <t>Le funzioni del sistema offerte al \uline{Dipendente} dovranno essere fruibili tramite interfaccia \uline{web}</t>
-  </si>
-  <si>
     <t>GENERALI</t>
   </si>
   <si>
@@ -200,12 +179,6 @@
     <t>RFD</t>
   </si>
   <si>
-    <t>Il sistema assegnerà in automatico badge/trofei al \uline{Dipendente}, quando questo raggiunge determinati obiettivi di \uline{Gamification}</t>
-  </si>
-  <si>
-    <t>Verbale 26/01/2012</t>
-  </si>
-  <si>
     <t>RFD .1</t>
   </si>
   <si>
@@ -272,9 +245,6 @@
     <t>Le domande che verranno sottoposte ai \uline{Dipendenti Autenticati} dovranno essere di tipologia diversa</t>
   </si>
   <si>
-    <t>Le domande che verranno sottoposte ai \uline{Dipendenti Autenticati} potranno avere risposta direttamente dalla propria postazione di lavoro</t>
-  </si>
-  <si>
     <t xml:space="preserve">Le domande a cui verranno sottoposti i \uline{Dipendenti Autenticati} forniti di \uline{dispositivi mobili} aziendali potranno prevedere delle prove pratiche </t>
   </si>
   <si>
@@ -299,9 +269,6 @@
     <t>La natura delle domande a cui verranno sottoposti i \uline{Dipendenti Autenticati} potrà variare a seconda dell'impiego dello stesso</t>
   </si>
   <si>
-    <t>Verbale 05/12/2011</t>
-  </si>
-  <si>
     <t>RFD .2.1</t>
   </si>
   <si>
@@ -329,9 +296,6 @@
     <t>UCDA 7</t>
   </si>
   <si>
-    <t>I dati personali visualizzabili sono: nome, cognome, codice fiscale, indirizzo di posta elettronica, impiego, password, username</t>
-  </si>
-  <si>
     <t>Un \uline{Dipendente Autenticato} a cui viene proposta la possibilità di rispondere ad una domanda potrà scegliere di visualizzarla e quindi rispondere, oppure rimandarla e rispondere successivamente</t>
   </si>
   <si>
@@ -434,9 +398,6 @@
     <t>Le statistiche personali sono: punti, trofei/badge</t>
   </si>
   <si>
-    <t>L'\uline{Amministratore Azienda Autenticato} dovrà poter modificare i badge/trofei di ogni singolo \uline{Dipendente}</t>
-  </si>
-  <si>
     <t>Un \uline{Amministratore Azienda Autenticato} dovrà avere la possibilità di terminare la propria sessione</t>
   </si>
   <si>
@@ -467,9 +428,6 @@
     <t>UCASA 3</t>
   </si>
   <si>
-    <t>Un \uline{Amministratore Sicurezza Autenticato} avrà la possibilità di aggiungere una domanda, dall'insieme di quelle già presenti nel database generale</t>
-  </si>
-  <si>
     <t>UCASA 3.1</t>
   </si>
   <si>
@@ -488,9 +446,6 @@
     <t>RFOP .1</t>
   </si>
   <si>
-    <t>L'\uline{Amministratore Sicurezza Autenticato} dovrà poter modificare i badge o trofei assegnabili agli utenti al raggiungimento di obiettivi di \uline{Gamification}</t>
-  </si>
-  <si>
     <t>Un \uline{Amministratore Sicurezza Autenticato} dovrà avere la possibilità di terminare la propria sessione</t>
   </si>
   <si>
@@ -525,6 +480,57 @@
   </si>
   <si>
     <t xml:space="preserve">Il sistema dovrà funzionare su qualsiasi \uline{dispositivo mobile} con sistema operativo \uline{Android} la cui versione è &gt;=1.6 e &lt;=4 </t>
+  </si>
+  <si>
+    <t>Le domande che verranno sottoposte ai \uline{Dipendenti Autenticati} potranno avere risposta direttamente dalla propria \uline{postazione di lavoro}</t>
+  </si>
+  <si>
+    <t>I dati personali visualizzabili sono: nome, cognome, codice fiscale, indirizzo di posta elettronica, impiego, username</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>RFOB .2.3</t>
+  </si>
+  <si>
+    <t>Il \uline{Dipendente} al primo accesso dovrà modificare la password</t>
+  </si>
+  <si>
+    <t>Un \uline{Amministratore Sicurezza Autenticato} avrà la possibilità di aggiungere una domanda dall'insieme di quelle già presenti nel database generale</t>
+  </si>
+  <si>
+    <t>Le funzioni del sistema offerte al \uline{Dipendente} dovranno essere anche fruibili tramite interfaccia \uline{web}</t>
+  </si>
+  <si>
+    <t>Sarà fornito un manuale ad uso dell'\uline{Amministratore Azienda}  riguardo tutte le azioni che potrà compiere</t>
+  </si>
+  <si>
+    <t>Sarà fornito un manuale ad uso dell'\uline{Amministratore Installatore} riguardo alle azioni che potrà compiere</t>
+  </si>
+  <si>
+    <t>Sarà fornito un manuale ad uso dell'\uline{Amministratore Sicurezza} riguardo le azioni che potrà compiere</t>
+  </si>
+  <si>
+    <t>Le applicazioni \uline{web} aderiranno allo standard \uline{W3C}</t>
+  </si>
+  <si>
+    <t>Verbale 2011/12/05</t>
+  </si>
+  <si>
+    <t>Verbale 2012/01/26</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>L'\uline{Amministratore Azienda Autenticato} dovrà poter modificare i trofei di ogni singolo \uline{Dipendente}</t>
+  </si>
+  <si>
+    <t>L'\uline{Amministratore Sicurezza Autenticato} dovrà poter modificare i badge assegnabili agli utenti al raggiungimento di obiettivi di \uline{Gamification}</t>
+  </si>
+  <si>
+    <t>Il sistema assegnerà in automatico i badge al \uline{Dipendente}, quando questo raggiunge determinati obiettivi di \uline{Gamification}</t>
   </si>
 </sst>
 </file>
@@ -568,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -586,6 +592,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -880,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="181.85546875" defaultRowHeight="15"/>
@@ -892,22 +899,23 @@
     <col min="2" max="2" width="209.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="16" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -916,12 +924,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -930,65 +938,74 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -997,12 +1014,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1011,93 +1028,93 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1106,12 +1123,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -1120,12 +1137,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1134,26 +1151,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1162,12 +1182,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1175,13 +1195,16 @@
       <c r="D23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -1190,12 +1213,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1204,12 +1227,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1218,12 +1241,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -1232,40 +1255,46 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>165</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>165</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
@@ -1274,12 +1303,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -1288,12 +1317,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
@@ -1302,12 +1331,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
@@ -1316,549 +1345,564 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" t="s">
         <v>101</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="D34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C36" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C38" t="s">
-        <v>108</v>
-      </c>
-      <c r="D38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" t="s">
-        <v>110</v>
-      </c>
-      <c r="D39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" t="s">
-        <v>110</v>
-      </c>
-      <c r="D40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="6" t="s">
-        <v>114</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C52" t="s">
         <v>116</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C53" t="s">
         <v>118</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C54" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="C55" t="s">
         <v>121</v>
       </c>
-      <c r="C47" t="s">
-        <v>120</v>
-      </c>
-      <c r="D47" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" s="1" t="s">
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C48" t="s">
-        <v>120</v>
-      </c>
-      <c r="D48" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
+      <c r="C56" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C57" t="s">
         <v>124</v>
       </c>
-      <c r="C49" t="s">
-        <v>120</v>
-      </c>
-      <c r="D49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C58" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C50" t="s">
-        <v>120</v>
-      </c>
-      <c r="D50" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="1" t="s">
+      <c r="C60" t="s">
         <v>127</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C63" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D52" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="1" t="s">
+      <c r="D63" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C53" t="s">
-        <v>130</v>
-      </c>
-      <c r="D53" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" s="1" t="s">
+      <c r="C64" t="s">
         <v>132</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15" customHeight="1">
+      <c r="A65" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D54" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="C65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C55" t="s">
-        <v>133</v>
-      </c>
-      <c r="D55" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="C66" t="s">
         <v>135</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D66" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>50</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C67" t="s">
         <v>136</v>
       </c>
-      <c r="D56" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="D67" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C57" t="s">
-        <v>136</v>
-      </c>
-      <c r="D57" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>75</v>
-      </c>
-      <c r="B58" s="1" t="s">
+      <c r="C68" t="s">
         <v>138</v>
       </c>
-      <c r="C58" t="s">
-        <v>136</v>
-      </c>
-      <c r="D58" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>75</v>
-      </c>
-      <c r="B59" s="1" t="s">
+      <c r="D68" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
         <v>139</v>
       </c>
-      <c r="C59" t="s">
+      <c r="B69" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D59" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="6" t="s">
+      <c r="C69" t="s">
+        <v>166</v>
+      </c>
+      <c r="D69" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
         <v>141</v>
       </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="B70" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C70" t="s">
+        <v>166</v>
+      </c>
+      <c r="D70" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C71" t="s">
         <v>143</v>
       </c>
-      <c r="D62" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
-        <v>55</v>
-      </c>
-      <c r="B63" s="1" t="s">
+      <c r="D71" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C63" t="s">
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D63" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1">
-      <c r="A64" t="s">
-        <v>57</v>
-      </c>
-      <c r="B64" s="1" t="s">
+      <c r="C74" t="s">
         <v>146</v>
       </c>
-      <c r="C64" t="s">
-        <v>145</v>
-      </c>
-      <c r="D64" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
-        <v>55</v>
-      </c>
-      <c r="B65" s="1" t="s">
+      <c r="D74" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>48</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C75" t="s">
         <v>148</v>
       </c>
-      <c r="D65" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
-        <v>57</v>
-      </c>
-      <c r="B66" s="1" t="s">
+      <c r="D75" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="C66" t="s">
-        <v>150</v>
-      </c>
-      <c r="D66" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" t="s">
-        <v>99</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C67" t="s">
-        <v>152</v>
-      </c>
-      <c r="D67" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" t="s">
-        <v>153</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C68" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
-        <v>155</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C69" t="s">
-        <v>61</v>
-      </c>
-      <c r="D69" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" t="s">
-        <v>55</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C70" t="s">
-        <v>158</v>
-      </c>
-      <c r="D70" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" t="s">
-        <v>55</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C73" t="s">
-        <v>161</v>
-      </c>
-      <c r="D73" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" t="s">
-        <v>55</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C74" t="s">
-        <v>163</v>
-      </c>
-      <c r="D74" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" t="s">
-        <v>55</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C75" t="s">
-        <v>18</v>
-      </c>
-      <c r="D75" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" t="s">
-        <v>55</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="C76" t="s">
         <v>18</v>
@@ -1867,12 +1911,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>153</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>166</v>
+        <v>48</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="C77" t="s">
         <v>18</v>
@@ -1881,75 +1925,98 @@
         <v>15</v>
       </c>
     </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>139</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" t="s">
+        <v>18</v>
+      </c>
+      <c r="D78" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A73:D73"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A62:D62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:B33"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="106.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1960,26 +2027,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="150.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -1988,12 +2055,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -2002,12 +2069,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -2016,12 +2083,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -2030,12 +2097,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -2043,13 +2110,16 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>163</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -2057,13 +2127,16 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -2071,13 +2144,16 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -2086,12 +2162,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -2100,12 +2176,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -2114,12 +2190,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -2128,12 +2204,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -2141,13 +2217,16 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -2156,12 +2235,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -2170,18 +2249,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2192,20 +2274,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="122.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2219,7 +2301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2233,7 +2315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2247,12 +2329,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -2261,7 +2343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2269,14 +2351,18 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2316,7 +2402,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Corretti errori ortografici PdP
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RQ/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
@@ -317,9 +317,6 @@
     <t>UCDA 5</t>
   </si>
   <si>
-    <t>Le informazioni che un \uline{Dipendente Autenticato} potrà consultare  sono: storico delle risposte (sia corrette che errate), classifica aziendale, trofei/badge raccolti, statistiche derivanti dalle risposte</t>
-  </si>
-  <si>
     <t>Un \uline{Dipendente Autenticato} dovrà avere la possibilità di terminare la propria sessione, senza chiudere l'applicazione</t>
   </si>
   <si>
@@ -395,9 +392,6 @@
     <t>UCAAA 4</t>
   </si>
   <si>
-    <t>Le statistiche personali sono: punti, trofei/badge</t>
-  </si>
-  <si>
     <t>Un \uline{Amministratore Azienda Autenticato} dovrà avere la possibilità di terminare la propria sessione</t>
   </si>
   <si>
@@ -531,6 +525,12 @@
   </si>
   <si>
     <t>Il sistema assegnerà in automatico i badge al \uline{Dipendente}, quando questo raggiunge determinati obiettivi di \uline{Gamification}</t>
+  </si>
+  <si>
+    <t>Le statistiche personali sono: punti, trofei e/o badge</t>
+  </si>
+  <si>
+    <t>Le informazioni che un \uline{Dipendente Autenticato} potrà consultare  sono: storico delle risposte (sia corrette che errate), classifica aziendale, trofei e/o badge raccolti, statistiche derivanti dalle risposte</t>
   </si>
 </sst>
 </file>
@@ -589,10 +589,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -890,7 +890,7 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="181.85546875" defaultRowHeight="15"/>
@@ -903,12 +903,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
@@ -943,16 +943,16 @@
         <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -963,13 +963,13 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -980,25 +980,25 @@
         <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
@@ -1074,12 +1074,12 @@
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
@@ -1159,13 +1159,13 @@
         <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1187,7 +1187,7 @@
         <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1196,7 +1196,7 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1263,13 +1263,13 @@
         <v>82</v>
       </c>
       <c r="C28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
         <v>165</v>
-      </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1280,13 +1280,13 @@
         <v>84</v>
       </c>
       <c r="C29" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
         <v>165</v>
-      </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1364,7 +1364,7 @@
         <v>50</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
@@ -1373,7 +1373,7 @@
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1437,7 +1437,7 @@
         <v>50</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="C40" t="s">
         <v>98</v>
@@ -1451,10 +1451,10 @@
         <v>48</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" t="s">
         <v>100</v>
-      </c>
-      <c r="C41" t="s">
-        <v>101</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
@@ -1464,22 +1464,22 @@
       <c r="B42" s="1"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
+      <c r="A43" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>15</v>
@@ -1490,10 +1490,10 @@
         <v>66</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>15</v>
@@ -1504,10 +1504,10 @@
         <v>48</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" t="s">
         <v>107</v>
-      </c>
-      <c r="C46" t="s">
-        <v>108</v>
       </c>
       <c r="D46" t="s">
         <v>15</v>
@@ -1518,10 +1518,10 @@
         <v>50</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -1532,10 +1532,10 @@
         <v>88</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D48" t="s">
         <v>15</v>
@@ -1543,13 +1543,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D49" t="s">
         <v>15</v>
@@ -1557,13 +1557,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" t="s">
         <v>15</v>
@@ -1571,19 +1571,19 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D51" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="7" t="s">
-        <v>156</v>
+      <c r="E51" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1591,10 +1591,10 @@
         <v>48</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" t="s">
         <v>115</v>
-      </c>
-      <c r="C52" t="s">
-        <v>116</v>
       </c>
       <c r="D52" t="s">
         <v>15</v>
@@ -1605,10 +1605,10 @@
         <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" t="s">
         <v>117</v>
-      </c>
-      <c r="C53" t="s">
-        <v>118</v>
       </c>
       <c r="D53" t="s">
         <v>15</v>
@@ -1619,10 +1619,10 @@
         <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
@@ -1633,10 +1633,10 @@
         <v>48</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" t="s">
         <v>120</v>
-      </c>
-      <c r="C55" t="s">
-        <v>121</v>
       </c>
       <c r="D55" t="s">
         <v>15</v>
@@ -1647,10 +1647,10 @@
         <v>50</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
@@ -1661,10 +1661,10 @@
         <v>48</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" t="s">
         <v>123</v>
-      </c>
-      <c r="C57" t="s">
-        <v>124</v>
       </c>
       <c r="D57" t="s">
         <v>15</v>
@@ -1675,10 +1675,10 @@
         <v>50</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>125</v>
+        <v>169</v>
       </c>
       <c r="C58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -1689,16 +1689,16 @@
         <v>66</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C59" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D59" t="s">
         <v>15</v>
       </c>
       <c r="E59" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1706,10 +1706,10 @@
         <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C60" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D60" t="s">
         <v>15</v>
@@ -1719,22 +1719,22 @@
       <c r="B61" s="1"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
+      <c r="A62" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>15</v>
@@ -1745,10 +1745,10 @@
         <v>48</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D64" t="s">
         <v>15</v>
@@ -1759,10 +1759,10 @@
         <v>50</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D65" t="s">
         <v>12</v>
@@ -1773,10 +1773,10 @@
         <v>48</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C66" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D66" t="s">
         <v>15</v>
@@ -1787,10 +1787,10 @@
         <v>50</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C67" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D67" t="s">
         <v>15</v>
@@ -1801,10 +1801,10 @@
         <v>88</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
         <v>15</v>
@@ -1812,36 +1812,36 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C69" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D69" t="s">
         <v>15</v>
       </c>
       <c r="E69" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C70" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D70" t="s">
         <v>15</v>
       </c>
       <c r="E70" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1849,10 +1849,10 @@
         <v>48</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C71" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D71" t="s">
         <v>15</v>
@@ -1862,22 +1862,22 @@
       <c r="B72" s="1"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
+      <c r="A73" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>48</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D74" t="s">
         <v>15</v>
@@ -1888,10 +1888,10 @@
         <v>48</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C75" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D75" t="s">
         <v>15</v>
@@ -1902,7 +1902,7 @@
         <v>48</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C76" t="s">
         <v>18</v>
@@ -1916,7 +1916,7 @@
         <v>48</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C77" t="s">
         <v>18</v>
@@ -1927,10 +1927,10 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C78" t="s">
         <v>18</v>
@@ -1982,7 +1982,7 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1999,7 +1999,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2007,7 +2007,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -2016,7 +2016,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2088,7 +2088,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -2102,7 +2102,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -2111,7 +2111,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2119,7 +2119,7 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -2128,7 +2128,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2145,7 +2145,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2209,7 +2209,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -2218,7 +2218,7 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2257,13 +2257,13 @@
         <v>43</v>
       </c>
       <c r="C15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
         <v>165</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2334,7 +2334,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -2351,13 +2351,13 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>165</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
up d modifiche varie e merge
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Analisi dei Requisiti/Requisiti.xlsx
+++ b/RQ/Esterni/Analisi dei Requisiti/Requisiti.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
@@ -317,9 +317,6 @@
     <t>UCDA 5</t>
   </si>
   <si>
-    <t>Le informazioni che un \uline{Dipendente Autenticato} potrà consultare  sono: storico delle risposte (sia corrette che errate), classifica aziendale, trofei/badge raccolti, statistiche derivanti dalle risposte</t>
-  </si>
-  <si>
     <t>Un \uline{Dipendente Autenticato} dovrà avere la possibilità di terminare la propria sessione, senza chiudere l'applicazione</t>
   </si>
   <si>
@@ -395,9 +392,6 @@
     <t>UCAAA 4</t>
   </si>
   <si>
-    <t>Le statistiche personali sono: punti, trofei/badge</t>
-  </si>
-  <si>
     <t>Un \uline{Amministratore Azienda Autenticato} dovrà avere la possibilità di terminare la propria sessione</t>
   </si>
   <si>
@@ -531,6 +525,12 @@
   </si>
   <si>
     <t>Il sistema assegnerà in automatico i badge al \uline{Dipendente}, quando questo raggiunge determinati obiettivi di \uline{Gamification}</t>
+  </si>
+  <si>
+    <t>Le statistiche personali sono: punti, trofei e/o badge</t>
+  </si>
+  <si>
+    <t>Le informazioni che un \uline{Dipendente Autenticato} potrà consultare  sono: storico delle risposte (sia corrette che errate), classifica aziendale, trofei e/o badge raccolti, statistiche derivanti dalle risposte</t>
   </si>
 </sst>
 </file>
@@ -589,10 +589,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -890,7 +890,7 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="181.85546875" defaultRowHeight="15"/>
@@ -903,12 +903,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
@@ -943,16 +943,16 @@
         <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -963,13 +963,13 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -980,25 +980,25 @@
         <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
@@ -1074,12 +1074,12 @@
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
@@ -1159,13 +1159,13 @@
         <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1187,7 +1187,7 @@
         <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1196,7 +1196,7 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1263,13 +1263,13 @@
         <v>82</v>
       </c>
       <c r="C28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
         <v>165</v>
-      </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1280,13 +1280,13 @@
         <v>84</v>
       </c>
       <c r="C29" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
         <v>165</v>
-      </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1364,7 +1364,7 @@
         <v>50</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C35" t="s">
         <v>91</v>
@@ -1373,7 +1373,7 @@
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1437,7 +1437,7 @@
         <v>50</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="C40" t="s">
         <v>98</v>
@@ -1451,10 +1451,10 @@
         <v>48</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" t="s">
         <v>100</v>
-      </c>
-      <c r="C41" t="s">
-        <v>101</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
@@ -1464,22 +1464,22 @@
       <c r="B42" s="1"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
+      <c r="A43" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>15</v>
@@ -1490,10 +1490,10 @@
         <v>66</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>15</v>
@@ -1504,10 +1504,10 @@
         <v>48</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" t="s">
         <v>107</v>
-      </c>
-      <c r="C46" t="s">
-        <v>108</v>
       </c>
       <c r="D46" t="s">
         <v>15</v>
@@ -1518,10 +1518,10 @@
         <v>50</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -1532,10 +1532,10 @@
         <v>88</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D48" t="s">
         <v>15</v>
@@ -1543,13 +1543,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D49" t="s">
         <v>15</v>
@@ -1557,13 +1557,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" t="s">
         <v>15</v>
@@ -1571,19 +1571,19 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D51" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="7" t="s">
-        <v>156</v>
+      <c r="E51" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1591,10 +1591,10 @@
         <v>48</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" t="s">
         <v>115</v>
-      </c>
-      <c r="C52" t="s">
-        <v>116</v>
       </c>
       <c r="D52" t="s">
         <v>15</v>
@@ -1605,10 +1605,10 @@
         <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" t="s">
         <v>117</v>
-      </c>
-      <c r="C53" t="s">
-        <v>118</v>
       </c>
       <c r="D53" t="s">
         <v>15</v>
@@ -1619,10 +1619,10 @@
         <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
@@ -1633,10 +1633,10 @@
         <v>48</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" t="s">
         <v>120</v>
-      </c>
-      <c r="C55" t="s">
-        <v>121</v>
       </c>
       <c r="D55" t="s">
         <v>15</v>
@@ -1647,10 +1647,10 @@
         <v>50</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
@@ -1661,10 +1661,10 @@
         <v>48</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" t="s">
         <v>123</v>
-      </c>
-      <c r="C57" t="s">
-        <v>124</v>
       </c>
       <c r="D57" t="s">
         <v>15</v>
@@ -1675,10 +1675,10 @@
         <v>50</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>125</v>
+        <v>169</v>
       </c>
       <c r="C58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -1689,16 +1689,16 @@
         <v>66</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C59" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D59" t="s">
         <v>15</v>
       </c>
       <c r="E59" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1706,10 +1706,10 @@
         <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C60" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D60" t="s">
         <v>15</v>
@@ -1719,22 +1719,22 @@
       <c r="B61" s="1"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
+      <c r="A62" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>15</v>
@@ -1745,10 +1745,10 @@
         <v>48</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D64" t="s">
         <v>15</v>
@@ -1759,10 +1759,10 @@
         <v>50</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D65" t="s">
         <v>12</v>
@@ -1773,10 +1773,10 @@
         <v>48</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C66" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D66" t="s">
         <v>15</v>
@@ -1787,10 +1787,10 @@
         <v>50</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C67" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D67" t="s">
         <v>15</v>
@@ -1801,10 +1801,10 @@
         <v>88</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
         <v>15</v>
@@ -1812,36 +1812,36 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C69" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D69" t="s">
         <v>15</v>
       </c>
       <c r="E69" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C70" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D70" t="s">
         <v>15</v>
       </c>
       <c r="E70" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1849,10 +1849,10 @@
         <v>48</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C71" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D71" t="s">
         <v>15</v>
@@ -1862,22 +1862,22 @@
       <c r="B72" s="1"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
+      <c r="A73" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>48</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D74" t="s">
         <v>15</v>
@@ -1888,10 +1888,10 @@
         <v>48</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C75" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D75" t="s">
         <v>15</v>
@@ -1902,7 +1902,7 @@
         <v>48</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C76" t="s">
         <v>18</v>
@@ -1916,7 +1916,7 @@
         <v>48</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C77" t="s">
         <v>18</v>
@@ -1927,10 +1927,10 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C78" t="s">
         <v>18</v>
@@ -1982,7 +1982,7 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1999,7 +1999,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2007,7 +2007,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -2016,7 +2016,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2088,7 +2088,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -2102,7 +2102,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -2111,7 +2111,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2119,7 +2119,7 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -2128,7 +2128,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2145,7 +2145,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2209,7 +2209,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -2218,7 +2218,7 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2257,13 +2257,13 @@
         <v>43</v>
       </c>
       <c r="C15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
         <v>165</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2334,7 +2334,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -2351,13 +2351,13 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>165</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>

</xml_diff>